<commit_message>
chore: Optimize fetching annonces based on createur and idList
</commit_message>
<xml_diff>
--- a/python/crenodataset.xlsx
+++ b/python/crenodataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -814,7 +814,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>10 - Bouira</t>
+          <t>Bouira</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -825,6 +825,52 @@
       <c r="E17" t="inlineStr">
         <is>
           <t>66530bad9acc7c37743889b2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>23</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>666317ac09c6d4281f17aa37</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>23</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>27 - Mostaganem</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Ain Tedeles</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>666317f909c6d4281f17aa3a</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: Update superficie field in terrain model
</commit_message>
<xml_diff>
--- a/python/crenodataset.xlsx
+++ b/python/crenodataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -860,7 +860,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>27 - Mostaganem</t>
+          <t>Mostaganem</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -871,6 +871,98 @@
       <c r="E19" t="inlineStr">
         <is>
           <t>666317f909c6d4281f17aa3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>23</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>6663b990f18db5d19ddbc69b</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>24</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>6663ba09f18db5d19ddbc69f</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>24</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>6663c158114e26a841e7b707</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>24</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>25 - Constantine</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>6663c30a114e26a841e7b86f</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: Update MongoDB connection in app.js to use environment variable for MongoURI and fix push notification controller
</commit_message>
<xml_diff>
--- a/python/crenodataset.xlsx
+++ b/python/crenodataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -952,17 +952,40 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>6663c30a114e26a841e7b86f</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>23</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>25 - Constantine</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Constantine</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>6663c30a114e26a841e7b86f</t>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>El Khroub</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>66670db52263a5b994b21f58</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: Update push notification controller to use correct screen name ,fix py
</commit_message>
<xml_diff>
--- a/python/crenodataset.xlsx
+++ b/python/crenodataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -989,6 +989,98 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>24</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Ibn Ziad</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>66677dd8d12a2002d45edd0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>24</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Ain Abid</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>66677ea9d12a2002d45edd33</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>24</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Ibn Ziad</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>66677f04d12a2002d45edd41</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>24</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>El Khroub</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>66677f75d12a2002d45edd54</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>